<commit_message>
Add commit file changes only
</commit_message>
<xml_diff>
--- a/commit_test.xlsx
+++ b/commit_test.xlsx
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>1º Teste</t>
   </si>
   <si>
     <t>commit</t>
+  </si>
+  <si>
+    <t>2º Teste</t>
+  </si>
+  <si>
+    <t>novo commit</t>
   </si>
 </sst>
 </file>
@@ -353,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:C3"/>
+  <dimension ref="B3:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -369,6 +375,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>